<commit_message>
Update iterations and times
</commit_message>
<xml_diff>
--- a/project time line and iteration estimates.xlsx
+++ b/project time line and iteration estimates.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="60">
   <si>
     <t xml:space="preserve">Tasks: </t>
   </si>
@@ -192,6 +192,21 @@
   </si>
   <si>
     <t xml:space="preserve">ebay/craiglist api </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mile stone 1 </t>
+  </si>
+  <si>
+    <t>Mile stone 2</t>
+  </si>
+  <si>
+    <t>Mile stone 3</t>
+  </si>
+  <si>
+    <t>(2 weeks)</t>
+  </si>
+  <si>
+    <t>(3 weeks)</t>
   </si>
 </sst>
 </file>
@@ -511,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -521,6 +536,24 @@
       <c r="B2" t="s">
         <v>0</v>
       </c>
+      <c r="F2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2" t="s">
+        <v>58</v>
+      </c>
+      <c r="M2" t="s">
+        <v>57</v>
+      </c>
+      <c r="N2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B3" t="s">

</xml_diff>